<commit_message>
changed calculated table product after change of specification source table stock
</commit_message>
<xml_diff>
--- a/Ekfa How to retrieve products that are in waiting to arrive mode/Ekfa How to retrieve products that are in waiting to arrive mode.xlsx
+++ b/Ekfa How to retrieve products that are in waiting to arrive mode/Ekfa How to retrieve products that are in waiting to arrive mode.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sergio\Dropbox\My PC (FROBOZZ)\Documents\GitHub\shared\Ekfa How to retrieve products that are in waiting to arrive mode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CBAE1BA-F276-444C-BFD6-7C7587D9788E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{821120BF-4BBD-49E6-B2DE-D8FFC997326B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2484" yWindow="1980" windowWidth="12588" windowHeight="10320" xr2:uid="{A6A901C9-A8DC-4E6D-8C46-49E7114E9788}"/>
+    <workbookView xWindow="1080" yWindow="312" windowWidth="21096" windowHeight="11748" xr2:uid="{A6A901C9-A8DC-4E6D-8C46-49E7114E9788}"/>
   </bookViews>
   <sheets>
     <sheet name="Tables" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="24">
   <si>
     <t>ID</t>
   </si>
@@ -106,12 +106,6 @@
   </si>
   <si>
     <t>stock</t>
-  </si>
-  <si>
-    <t>body oil</t>
-  </si>
-  <si>
-    <t>perfume</t>
   </si>
 </sst>
 </file>
@@ -200,16 +194,15 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{70B329E4-4D33-4CA5-B936-FA37F7515496}" name="Stock" displayName="Stock" ref="M1:Q8" totalsRowShown="0">
-  <autoFilter ref="M1:Q8" xr:uid="{25872EA3-3FF8-4608-B92A-3A033E1A271D}"/>
-  <tableColumns count="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{70B329E4-4D33-4CA5-B936-FA37F7515496}" name="Stock" displayName="Stock" ref="M1:P8" totalsRowShown="0">
+  <autoFilter ref="M1:P8" xr:uid="{25872EA3-3FF8-4608-B92A-3A033E1A271D}"/>
+  <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{ADC9F419-8038-4D1B-925D-F90CAAF1E453}" name="ID">
       <calculatedColumnFormula>M1+1</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="2" xr3:uid="{F3762866-CC45-4C18-BB12-57E6F238F94D}" name="EAN"/>
     <tableColumn id="3" xr3:uid="{0B7CA089-7628-493A-B57D-765DA8D19575}" name="Ordernumber"/>
     <tableColumn id="4" xr3:uid="{368067EF-52B5-49B6-AE39-6A34B628E242}" name="Location"/>
-    <tableColumn id="5" xr3:uid="{3C70F808-1C42-4AB2-9AD8-2B2BDD821AA3}" name="Product"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -512,10 +505,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0102A0C8-ED90-493B-B031-73ED69C0C51E}">
-  <dimension ref="A1:Q8"/>
+  <dimension ref="A1:P8"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+      <selection activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -529,10 +522,9 @@
     <col min="14" max="14" width="10" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="14.33203125" customWidth="1"/>
     <col min="16" max="16" width="10.109375" customWidth="1"/>
-    <col min="17" max="17" width="9.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -575,11 +567,8 @@
       <c r="P1" t="s">
         <v>20</v>
       </c>
-      <c r="Q1" t="s">
-        <v>14</v>
-      </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>12345</v>
       </c>
@@ -622,11 +611,8 @@
       <c r="P2" t="s">
         <v>21</v>
       </c>
-      <c r="Q2" t="s">
-        <v>17</v>
-      </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>12346</v>
       </c>
@@ -669,11 +655,8 @@
       <c r="P3" t="s">
         <v>21</v>
       </c>
-      <c r="Q3" t="s">
-        <v>17</v>
-      </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>12347</v>
       </c>
@@ -716,11 +699,8 @@
       <c r="P4" t="s">
         <v>22</v>
       </c>
-      <c r="Q4" t="s">
-        <v>18</v>
-      </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="G5">
         <v>8768</v>
       </c>
@@ -749,11 +729,8 @@
       <c r="P5" t="s">
         <v>22</v>
       </c>
-      <c r="Q5" t="s">
-        <v>18</v>
-      </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="G6">
         <v>8769</v>
       </c>
@@ -779,11 +756,8 @@
       <c r="P6" t="s">
         <v>23</v>
       </c>
-      <c r="Q6" t="s">
-        <v>24</v>
-      </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="M7">
         <f t="shared" si="0"/>
         <v>5555560</v>
@@ -794,11 +768,8 @@
       <c r="P7" t="s">
         <v>23</v>
       </c>
-      <c r="Q7" t="s">
-        <v>25</v>
-      </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="M8">
         <f t="shared" si="0"/>
         <v>5555561</v>
@@ -808,9 +779,6 @@
       </c>
       <c r="P8" t="s">
         <v>23</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>